<commit_message>
Converted Maze to .csv fie for reading, started working on JUnit testing for the Maze
</commit_message>
<xml_diff>
--- a/Maze.xlsx
+++ b/Maze.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="192" yWindow="108" windowWidth="17220" windowHeight="6888"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Maze" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,9 +16,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="15">
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -34,7 +76,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -50,6 +92,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -71,8 +119,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -376,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX50"/>
+  <dimension ref="A1:AH34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -387,7 +437,7 @@
     <col min="1" max="50" width="4.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,170 +540,122 @@
       <c r="AH1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AI1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
-        <v>0</v>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3">
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
         <v>0</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="3">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>0</v>
-      </c>
-      <c r="N2" s="3">
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2">
         <v>0</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>0</v>
-      </c>
-      <c r="R2" s="3">
-        <v>0</v>
-      </c>
-      <c r="S2" s="3">
-        <v>0</v>
-      </c>
-      <c r="T2" s="3">
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2">
         <v>0</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V2" s="3">
-        <v>0</v>
-      </c>
-      <c r="W2" s="3">
-        <v>0</v>
-      </c>
-      <c r="X2" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="3">
+      <c r="V2" s="2">
+        <v>0</v>
+      </c>
+      <c r="W2" s="2">
+        <v>0</v>
+      </c>
+      <c r="X2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="2">
         <v>0</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AC2" s="3">
+      <c r="AC2" s="2">
         <v>0</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AE2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="3">
+      <c r="AE2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="2">
         <v>0</v>
       </c>
       <c r="AH2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -662,7 +664,7 @@
       <c r="F3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -677,13 +679,13 @@
       <c r="K3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="2">
         <v>0</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="2">
         <v>0</v>
       </c>
       <c r="O3" s="1" t="s">
@@ -701,19 +703,19 @@
       <c r="S3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T3" s="3">
+      <c r="T3" s="2">
         <v>0</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V3" s="3">
+      <c r="V3" s="2">
         <v>0</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X3" s="3">
+      <c r="X3" s="2">
         <v>0</v>
       </c>
       <c r="Y3" s="1" t="s">
@@ -728,90 +730,90 @@
       <c r="AB3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AC3" s="2">
         <v>0</v>
       </c>
       <c r="AD3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AE3" s="3">
+      <c r="AE3" s="2">
         <v>0</v>
       </c>
       <c r="AF3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG3" s="3">
+      <c r="AG3" s="2">
         <v>0</v>
       </c>
       <c r="AH3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
         <v>0</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="3">
-        <v>0</v>
-      </c>
-      <c r="O4" s="3">
-        <v>0</v>
-      </c>
-      <c r="P4" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>0</v>
-      </c>
-      <c r="R4" s="3">
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
         <v>0</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T4" s="3">
+      <c r="T4" s="2">
         <v>0</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V4" s="3">
+      <c r="V4" s="2">
         <v>0</v>
       </c>
       <c r="W4" s="1" t="s">
@@ -823,39 +825,39 @@
       <c r="Y4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z4" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="3">
+      <c r="Z4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="2">
         <v>0</v>
       </c>
       <c r="AD4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AE4" s="3">
+      <c r="AE4" s="2">
         <v>0</v>
       </c>
       <c r="AF4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG4" s="3">
+      <c r="AG4" s="2">
         <v>0</v>
       </c>
       <c r="AH4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -864,13 +866,13 @@
       <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -879,7 +881,7 @@
       <c r="I5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>0</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -891,7 +893,7 @@
       <c r="M5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>0</v>
       </c>
       <c r="O5" s="1" t="s">
@@ -903,37 +905,37 @@
       <c r="Q5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R5" s="3">
-        <v>0</v>
-      </c>
-      <c r="S5" s="3">
-        <v>0</v>
-      </c>
-      <c r="T5" s="3">
-        <v>0</v>
-      </c>
-      <c r="U5" s="3">
-        <v>0</v>
-      </c>
-      <c r="V5" s="3">
-        <v>0</v>
-      </c>
-      <c r="W5" s="3">
-        <v>0</v>
-      </c>
-      <c r="X5" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="3">
+      <c r="R5" s="2">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2">
+        <v>0</v>
+      </c>
+      <c r="W5" s="2">
+        <v>0</v>
+      </c>
+      <c r="X5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="2">
         <v>0</v>
       </c>
       <c r="AA5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB5" s="3">
+      <c r="AB5" s="2">
         <v>0</v>
       </c>
       <c r="AC5" s="1" t="s">
@@ -942,72 +944,72 @@
       <c r="AD5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AE5" s="3">
+      <c r="AE5" s="2">
         <v>0</v>
       </c>
       <c r="AF5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG5" s="3">
+      <c r="AG5" s="2">
         <v>0</v>
       </c>
       <c r="AH5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>0</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="2">
         <v>0</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="2">
         <v>0</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="2">
         <v>0</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R6" s="3">
+      <c r="R6" s="2">
         <v>0</v>
       </c>
       <c r="S6" s="1" t="s">
@@ -1019,7 +1021,7 @@
       <c r="U6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V6" s="3">
+      <c r="V6" s="2">
         <v>0</v>
       </c>
       <c r="W6" s="1" t="s">
@@ -1031,39 +1033,39 @@
       <c r="Y6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z6" s="3">
+      <c r="Z6" s="2">
         <v>0</v>
       </c>
       <c r="AA6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB6" s="3">
+      <c r="AB6" s="2">
         <v>0</v>
       </c>
       <c r="AC6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AD6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="3">
+      <c r="AD6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE6" s="2">
         <v>0</v>
       </c>
       <c r="AF6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG6" s="3">
+      <c r="AG6" s="2">
         <v>0</v>
       </c>
       <c r="AH6" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1081,67 +1083,67 @@
       <c r="G7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>0</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <v>0</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N7" s="3">
-        <v>0</v>
-      </c>
-      <c r="O7" s="3">
-        <v>0</v>
-      </c>
-      <c r="P7" s="3">
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
         <v>0</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R7" s="3">
+      <c r="R7" s="2">
         <v>0</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T7" s="3">
-        <v>0</v>
+      <c r="T7" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V7" s="3">
+      <c r="V7" s="2">
         <v>0</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X7" s="3">
+      <c r="X7" s="2">
         <v>0</v>
       </c>
       <c r="Y7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z7" s="3">
+      <c r="Z7" s="2">
         <v>0</v>
       </c>
       <c r="AA7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB7" s="3">
+      <c r="AB7" s="2">
         <v>0</v>
       </c>
       <c r="AC7" s="1" t="s">
@@ -1156,14 +1158,14 @@
       <c r="AF7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG7" s="3">
+      <c r="AG7" s="2">
         <v>0</v>
       </c>
       <c r="AH7" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1173,37 +1175,37 @@
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>0</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="2">
         <v>0</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="2">
         <v>0</v>
       </c>
       <c r="O8" s="1" t="s">
@@ -1215,123 +1217,123 @@
       <c r="Q8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R8" s="3">
+      <c r="R8" s="2">
         <v>0</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T8" s="3">
+      <c r="T8" s="2">
         <v>0</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V8" s="3">
+      <c r="V8" s="2">
         <v>0</v>
       </c>
       <c r="W8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X8" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="3">
+      <c r="X8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="2">
         <v>0</v>
       </c>
       <c r="AA8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB8" s="3">
+      <c r="AB8" s="2">
         <v>0</v>
       </c>
       <c r="AC8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AD8" s="3">
+      <c r="AD8" s="2">
         <v>0</v>
       </c>
       <c r="AE8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AF8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="3">
+      <c r="AF8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="2">
         <v>0</v>
       </c>
       <c r="AH8" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
         <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3">
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
         <v>0</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="2">
         <v>0</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P9" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="3">
-        <v>0</v>
-      </c>
-      <c r="R9" s="3">
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
         <v>0</v>
       </c>
       <c r="S9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T9" s="3">
+      <c r="T9" s="2">
         <v>0</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V9" s="3">
+      <c r="V9" s="2">
         <v>0</v>
       </c>
       <c r="W9" s="1" t="s">
@@ -1343,39 +1345,39 @@
       <c r="Y9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z9" s="3">
+      <c r="Z9" s="2">
         <v>0</v>
       </c>
       <c r="AA9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="3">
+      <c r="AB9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="2">
         <v>0</v>
       </c>
       <c r="AH9" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1387,7 +1389,7 @@
       <c r="E10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1405,19 +1407,19 @@
       <c r="K10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="2">
         <v>0</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="2">
         <v>0</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10" s="2">
         <v>0</v>
       </c>
       <c r="Q10" s="1" t="s">
@@ -1429,25 +1431,25 @@
       <c r="S10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T10" s="3">
+      <c r="T10" s="2">
         <v>0</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V10" s="3">
+      <c r="V10" s="2">
         <v>0</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X10" s="3">
+      <c r="X10" s="2">
         <v>0</v>
       </c>
       <c r="Y10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z10" s="3">
+      <c r="Z10" s="2">
         <v>0</v>
       </c>
       <c r="AA10" s="1" t="s">
@@ -1475,53 +1477,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="3">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3">
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="3">
-        <v>0</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0</v>
-      </c>
-      <c r="J11" s="3">
+      <c r="H11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
         <v>0</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L11" s="3">
-        <v>0</v>
+      <c r="L11" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="2">
         <v>0</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P11" s="3">
+      <c r="P11" s="2">
         <v>0</v>
       </c>
       <c r="Q11" s="1" t="s">
@@ -1533,28 +1535,28 @@
       <c r="S11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T11" s="3">
+      <c r="T11" s="2">
         <v>0</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V11" s="3">
+      <c r="V11" s="2">
         <v>0</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X11" s="3">
+      <c r="X11" s="2">
         <v>0</v>
       </c>
       <c r="Y11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="3">
+      <c r="Z11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="2">
         <v>0</v>
       </c>
       <c r="AB11" s="1" t="s">
@@ -1563,27 +1565,27 @@
       <c r="AC11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AD11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="3">
+      <c r="AD11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="2">
         <v>0</v>
       </c>
       <c r="AH11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1595,7 +1597,7 @@
       <c r="E12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1607,7 +1609,7 @@
       <c r="I12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <v>0</v>
       </c>
       <c r="K12" s="1" t="s">
@@ -1625,43 +1627,43 @@
       <c r="O12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12" s="2">
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R12" s="3">
-        <v>0</v>
-      </c>
-      <c r="S12" s="3">
-        <v>0</v>
-      </c>
-      <c r="T12" s="3">
+      <c r="R12" s="2">
+        <v>0</v>
+      </c>
+      <c r="S12" s="2">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2">
         <v>0</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V12" s="3">
-        <v>0</v>
-      </c>
-      <c r="W12" s="3">
-        <v>0</v>
-      </c>
-      <c r="X12" s="3">
+      <c r="V12" s="2">
+        <v>0</v>
+      </c>
+      <c r="W12" s="2">
+        <v>0</v>
+      </c>
+      <c r="X12" s="2">
         <v>0</v>
       </c>
       <c r="Y12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z12" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="3">
+      <c r="Z12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="2">
         <v>0</v>
       </c>
       <c r="AC12" s="1" t="s">
@@ -1676,66 +1678,66 @@
       <c r="AF12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG12" s="3">
+      <c r="AG12" s="2">
         <v>0</v>
       </c>
       <c r="AH12" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="3">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="3">
-        <v>0</v>
-      </c>
-      <c r="K13" s="3">
-        <v>0</v>
-      </c>
-      <c r="L13" s="3">
-        <v>0</v>
-      </c>
-      <c r="M13" s="3">
-        <v>0</v>
-      </c>
-      <c r="N13" s="3">
-        <v>0</v>
-      </c>
-      <c r="O13" s="3">
-        <v>0</v>
-      </c>
-      <c r="P13" s="3">
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
         <v>0</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R13" s="3">
+      <c r="R13" s="2">
         <v>0</v>
       </c>
       <c r="S13" s="1" t="s">
@@ -1759,45 +1761,45 @@
       <c r="Y13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z13" s="3">
+      <c r="Z13" s="2">
         <v>0</v>
       </c>
       <c r="AA13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB13" s="3">
+      <c r="AB13" s="2">
         <v>0</v>
       </c>
       <c r="AC13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AD13" s="3">
+      <c r="AD13" s="2">
         <v>0</v>
       </c>
       <c r="AE13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AF13" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="3">
+      <c r="AF13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="2">
         <v>0</v>
       </c>
       <c r="AH13" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -1809,7 +1811,7 @@
       <c r="G14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -1824,7 +1826,7 @@
       <c r="L14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M14" s="3">
+      <c r="M14" s="2">
         <v>0</v>
       </c>
       <c r="N14" s="1" t="s">
@@ -1833,55 +1835,55 @@
       <c r="O14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14" s="2">
         <v>0</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R14" s="3">
-        <v>0</v>
-      </c>
-      <c r="S14" s="3">
-        <v>0</v>
-      </c>
-      <c r="T14" s="3">
-        <v>0</v>
-      </c>
-      <c r="U14" s="3">
-        <v>0</v>
-      </c>
-      <c r="V14" s="3">
-        <v>0</v>
-      </c>
-      <c r="W14" s="3">
-        <v>0</v>
-      </c>
-      <c r="X14" s="3">
+      <c r="R14" s="2">
+        <v>0</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
+        <v>0</v>
+      </c>
+      <c r="U14" s="2">
+        <v>0</v>
+      </c>
+      <c r="V14" s="2">
+        <v>0</v>
+      </c>
+      <c r="W14" s="2">
+        <v>0</v>
+      </c>
+      <c r="X14" s="2">
         <v>0</v>
       </c>
       <c r="Y14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z14" s="3">
+      <c r="Z14" s="2">
         <v>0</v>
       </c>
       <c r="AA14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB14" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="3">
+      <c r="AB14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="2">
         <v>0</v>
       </c>
       <c r="AG14" s="1" t="s">
@@ -1891,59 +1893,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="3">
-        <v>0</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0</v>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3">
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="3">
-        <v>0</v>
-      </c>
-      <c r="K15" s="3">
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
         <v>0</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M15" s="3">
-        <v>0</v>
-      </c>
-      <c r="N15" s="3">
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
         <v>0</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P15" s="3">
+      <c r="P15" s="2">
         <v>0</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R15" s="3">
+      <c r="R15" s="2">
         <v>0</v>
       </c>
       <c r="S15" s="1" t="s">
@@ -1967,7 +1969,7 @@
       <c r="Y15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z15" s="3">
+      <c r="Z15" s="2">
         <v>0</v>
       </c>
       <c r="AA15" s="1" t="s">
@@ -1976,7 +1978,7 @@
       <c r="AB15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AC15" s="3">
+      <c r="AC15" s="2">
         <v>0</v>
       </c>
       <c r="AD15" s="1" t="s">
@@ -1995,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2017,13 +2019,13 @@
       <c r="G16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="2">
         <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <v>0</v>
       </c>
       <c r="K16" s="1" t="s">
@@ -2035,64 +2037,64 @@
       <c r="M16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16" s="2">
         <v>0</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P16" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>0</v>
-      </c>
-      <c r="R16" s="3">
+      <c r="P16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>0</v>
+      </c>
+      <c r="R16" s="2">
         <v>0</v>
       </c>
       <c r="S16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T16" s="3">
-        <v>0</v>
-      </c>
-      <c r="U16" s="3">
-        <v>0</v>
-      </c>
-      <c r="V16" s="3">
-        <v>0</v>
-      </c>
-      <c r="W16" s="3">
-        <v>0</v>
-      </c>
-      <c r="X16" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="3">
+      <c r="T16" s="2">
+        <v>0</v>
+      </c>
+      <c r="U16" s="2">
+        <v>0</v>
+      </c>
+      <c r="V16" s="2">
+        <v>0</v>
+      </c>
+      <c r="W16" s="2">
+        <v>0</v>
+      </c>
+      <c r="X16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="2">
         <v>0</v>
       </c>
       <c r="AB16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AC16" s="3">
+      <c r="AC16" s="2">
         <v>0</v>
       </c>
       <c r="AD16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AE16" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF16" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG16" s="3">
+      <c r="AE16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="2">
         <v>0</v>
       </c>
       <c r="AH16" s="1" t="s">
@@ -2103,13 +2105,13 @@
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="3">
-        <v>0</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3">
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -2121,31 +2123,31 @@
       <c r="G17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="2">
         <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="2">
         <v>0</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L17" s="3">
-        <v>0</v>
+      <c r="L17" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N17" s="2">
         <v>0</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P17" s="3">
+      <c r="P17" s="2">
         <v>0</v>
       </c>
       <c r="Q17" s="1" t="s">
@@ -2157,22 +2159,22 @@
       <c r="S17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T17" s="3">
+      <c r="T17" s="2">
         <v>0</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V17" s="3">
+      <c r="V17" s="2">
         <v>0</v>
       </c>
       <c r="W17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X17" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="3">
+      <c r="X17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="2">
         <v>0</v>
       </c>
       <c r="Z17" s="1" t="s">
@@ -2184,19 +2186,19 @@
       <c r="AB17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AC17" s="3">
+      <c r="AC17" s="2">
         <v>0</v>
       </c>
       <c r="AD17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AE17" s="3">
+      <c r="AE17" s="2">
         <v>0</v>
       </c>
       <c r="AF17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG17" s="3">
+      <c r="AG17" s="2">
         <v>0</v>
       </c>
       <c r="AH17" s="1" t="s">
@@ -2207,7 +2209,7 @@
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2219,56 +2221,56 @@
       <c r="E18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0</v>
-      </c>
-      <c r="I18" s="3">
-        <v>0</v>
-      </c>
-      <c r="J18" s="3">
-        <v>0</v>
-      </c>
-      <c r="K18" s="3">
-        <v>0</v>
-      </c>
-      <c r="L18" s="3">
-        <v>0</v>
-      </c>
-      <c r="M18" s="3">
-        <v>0</v>
-      </c>
-      <c r="N18" s="3">
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2">
         <v>0</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P18" s="3">
+      <c r="P18" s="2">
         <v>0</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R18" s="3">
+      <c r="R18" s="2">
         <v>0</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T18" s="3">
+      <c r="T18" s="2">
         <v>0</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V18" s="3">
-        <v>0</v>
+      <c r="V18" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>0</v>
@@ -2276,31 +2278,31 @@
       <c r="X18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Y18" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD18" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="3">
+      <c r="Y18" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="2">
         <v>0</v>
       </c>
       <c r="AF18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG18" s="3">
+      <c r="AG18" s="2">
         <v>0</v>
       </c>
       <c r="AH18" s="1" t="s">
@@ -2311,25 +2313,25 @@
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="3">
-        <v>0</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0</v>
-      </c>
-      <c r="F19" s="3">
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
         <v>0</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -2353,13 +2355,13 @@
       <c r="O19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P19" s="3">
+      <c r="P19" s="2">
         <v>0</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R19" s="3">
+      <c r="R19" s="2">
         <v>0</v>
       </c>
       <c r="S19" s="1" t="s">
@@ -2377,22 +2379,22 @@
       <c r="W19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X19" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="3">
+      <c r="X19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="2">
         <v>0</v>
       </c>
       <c r="Z19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AA19" s="3">
+      <c r="AA19" s="2">
         <v>0</v>
       </c>
       <c r="AB19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AC19" s="3">
+      <c r="AC19" s="2">
         <v>0</v>
       </c>
       <c r="AD19" s="1" t="s">
@@ -2404,7 +2406,7 @@
       <c r="AF19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG19" s="3">
+      <c r="AG19" s="2">
         <v>0</v>
       </c>
       <c r="AH19" s="1" t="s">
@@ -2415,7 +2417,7 @@
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2433,55 +2435,55 @@
       <c r="G20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H20" s="3">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
-        <v>0</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0</v>
-      </c>
-      <c r="K20" s="3">
-        <v>0</v>
-      </c>
-      <c r="L20" s="3">
-        <v>0</v>
-      </c>
-      <c r="M20" s="3">
-        <v>0</v>
-      </c>
-      <c r="N20" s="3">
-        <v>0</v>
-      </c>
-      <c r="O20" s="3">
-        <v>0</v>
-      </c>
-      <c r="P20" s="3">
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2">
+        <v>0</v>
+      </c>
+      <c r="O20" s="2">
+        <v>0</v>
+      </c>
+      <c r="P20" s="2">
         <v>0</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R20" s="3">
-        <v>0</v>
-      </c>
-      <c r="S20" s="3">
-        <v>0</v>
-      </c>
-      <c r="T20" s="3">
-        <v>0</v>
-      </c>
-      <c r="U20" s="3">
-        <v>0</v>
-      </c>
-      <c r="V20" s="3">
+      <c r="R20" s="2">
+        <v>0</v>
+      </c>
+      <c r="S20" s="2">
+        <v>0</v>
+      </c>
+      <c r="T20" s="2">
+        <v>0</v>
+      </c>
+      <c r="U20" s="2">
+        <v>0</v>
+      </c>
+      <c r="V20" s="2">
         <v>0</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X20" s="3">
+      <c r="X20" s="2">
         <v>0</v>
       </c>
       <c r="Y20" s="1" t="s">
@@ -2490,25 +2492,25 @@
       <c r="Z20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AA20" s="3">
+      <c r="AA20" s="2">
         <v>0</v>
       </c>
       <c r="AB20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AC20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE20" s="3">
+      <c r="AC20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="2">
         <v>0</v>
       </c>
       <c r="AF20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG20" s="3">
+      <c r="AG20" s="2">
         <v>0</v>
       </c>
       <c r="AH20" s="1" t="s">
@@ -2519,20 +2521,20 @@
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>0</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F21" s="3">
-        <v>0</v>
+      <c r="F21" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>0</v>
@@ -2540,13 +2542,13 @@
       <c r="H21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="2">
         <v>0</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21" s="2">
         <v>0</v>
       </c>
       <c r="L21" s="1" t="s">
@@ -2561,13 +2563,13 @@
       <c r="O21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P21" s="2">
         <v>0</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R21" s="3">
+      <c r="R21" s="2">
         <v>0</v>
       </c>
       <c r="S21" s="1" t="s">
@@ -2579,22 +2581,22 @@
       <c r="U21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V21" s="3">
+      <c r="V21" s="2">
         <v>0</v>
       </c>
       <c r="W21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X21" s="3">
+      <c r="X21" s="2">
         <v>0</v>
       </c>
       <c r="Y21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z21" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA21" s="3">
+      <c r="Z21" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="2">
         <v>0</v>
       </c>
       <c r="AB21" s="1" t="s">
@@ -2606,7 +2608,7 @@
       <c r="AD21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AE21" s="3">
+      <c r="AE21" s="2">
         <v>0</v>
       </c>
       <c r="AF21" s="1" t="s">
@@ -2629,28 +2631,28 @@
       <c r="C22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>0</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F22" s="3">
-        <v>0</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
         <v>0</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="2">
         <v>0</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K22" s="2">
         <v>0</v>
       </c>
       <c r="L22" s="1" t="s">
@@ -2662,34 +2664,34 @@
       <c r="N22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O22" s="3">
-        <v>0</v>
-      </c>
-      <c r="P22" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="3">
-        <v>0</v>
-      </c>
-      <c r="R22" s="3">
+      <c r="O22" s="2">
+        <v>0</v>
+      </c>
+      <c r="P22" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>0</v>
+      </c>
+      <c r="R22" s="2">
         <v>0</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T22" s="3">
-        <v>0</v>
+      <c r="T22" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="U22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V22" s="3">
+      <c r="V22" s="2">
         <v>0</v>
       </c>
       <c r="W22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X22" s="3">
+      <c r="X22" s="2">
         <v>0</v>
       </c>
       <c r="Y22" s="1" t="s">
@@ -2698,25 +2700,25 @@
       <c r="Z22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AA22" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="3">
+      <c r="AA22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="2">
         <v>0</v>
       </c>
       <c r="AC22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AD22" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE22" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF22" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG22" s="3">
+      <c r="AD22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="2">
         <v>0</v>
       </c>
       <c r="AH22" s="1" t="s">
@@ -2727,19 +2729,19 @@
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="3">
-        <v>0</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3">
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
         <v>0</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>0</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -2748,19 +2750,19 @@
       <c r="H23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <v>0</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K23" s="3">
-        <v>0</v>
-      </c>
-      <c r="L23" s="3">
-        <v>0</v>
-      </c>
-      <c r="M23" s="3">
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2">
         <v>0</v>
       </c>
       <c r="N23" s="1" t="s">
@@ -2775,28 +2777,28 @@
       <c r="Q23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R23" s="3">
+      <c r="R23" s="2">
         <v>0</v>
       </c>
       <c r="S23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T23" s="3">
-        <v>0</v>
-      </c>
-      <c r="U23" s="3">
-        <v>0</v>
-      </c>
-      <c r="V23" s="3">
+      <c r="T23" s="2">
+        <v>0</v>
+      </c>
+      <c r="U23" s="2">
+        <v>0</v>
+      </c>
+      <c r="V23" s="2">
         <v>0</v>
       </c>
       <c r="W23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X23" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="3">
+      <c r="X23" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="2">
         <v>0</v>
       </c>
       <c r="Z23" s="1" t="s">
@@ -2805,13 +2807,13 @@
       <c r="AA23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB23" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD23" s="3">
+      <c r="AB23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="2">
         <v>0</v>
       </c>
       <c r="AE23" s="1" t="s">
@@ -2831,7 +2833,7 @@
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -2843,16 +2845,16 @@
       <c r="E24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F24" s="3">
-        <v>0</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0</v>
-      </c>
-      <c r="H24" s="3">
-        <v>0</v>
-      </c>
-      <c r="I24" s="3">
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
         <v>0</v>
       </c>
       <c r="J24" s="1" t="s">
@@ -2861,25 +2863,25 @@
       <c r="K24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L24" s="3">
-        <v>0</v>
-      </c>
-      <c r="M24" s="3">
-        <v>0</v>
-      </c>
-      <c r="N24" s="3">
-        <v>0</v>
-      </c>
-      <c r="O24" s="3">
-        <v>0</v>
-      </c>
-      <c r="P24" s="3">
+      <c r="L24" s="2">
+        <v>0</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0</v>
+      </c>
+      <c r="N24" s="2">
+        <v>0</v>
+      </c>
+      <c r="O24" s="2">
+        <v>0</v>
+      </c>
+      <c r="P24" s="2">
         <v>0</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R24" s="3">
+      <c r="R24" s="2">
         <v>0</v>
       </c>
       <c r="S24" s="1" t="s">
@@ -2900,10 +2902,10 @@
       <c r="X24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Y24" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="3">
+      <c r="Y24" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="2">
         <v>0</v>
       </c>
       <c r="AA24" s="1" t="s">
@@ -2921,11 +2923,11 @@
       <c r="AE24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AF24" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG24" s="3">
-        <v>0</v>
+      <c r="AF24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="AH24" s="1" t="s">
         <v>0</v>
@@ -2935,19 +2937,19 @@
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="3">
-        <v>0</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0</v>
-      </c>
-      <c r="E25" s="3">
-        <v>0</v>
-      </c>
-      <c r="F25" s="3">
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -2965,7 +2967,7 @@
       <c r="K25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L25" s="2">
         <v>0</v>
       </c>
       <c r="M25" s="1" t="s">
@@ -2977,28 +2979,28 @@
       <c r="O25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P25" s="3">
+      <c r="P25" s="2">
         <v>0</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R25" s="3">
-        <v>0</v>
-      </c>
-      <c r="S25" s="3">
-        <v>0</v>
-      </c>
-      <c r="T25" s="3">
-        <v>0</v>
-      </c>
-      <c r="U25" s="3">
-        <v>0</v>
-      </c>
-      <c r="V25" s="3">
-        <v>0</v>
-      </c>
-      <c r="W25" s="3">
+      <c r="R25" s="2">
+        <v>0</v>
+      </c>
+      <c r="S25" s="2">
+        <v>0</v>
+      </c>
+      <c r="T25" s="2">
+        <v>0</v>
+      </c>
+      <c r="U25" s="2">
+        <v>0</v>
+      </c>
+      <c r="V25" s="2">
+        <v>0</v>
+      </c>
+      <c r="W25" s="2">
         <v>0</v>
       </c>
       <c r="X25" s="1" t="s">
@@ -3007,28 +3009,28 @@
       <c r="Y25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z25" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA25" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="3">
+      <c r="Z25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="2">
         <v>0</v>
       </c>
       <c r="AC25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AD25" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE25" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF25" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG25" s="3">
+      <c r="AD25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG25" s="2">
         <v>0</v>
       </c>
       <c r="AH25" s="1" t="s">
@@ -3039,7 +3041,7 @@
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -3051,61 +3053,61 @@
       <c r="E26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H26" s="3">
-        <v>0</v>
-      </c>
-      <c r="I26" s="3">
-        <v>0</v>
-      </c>
-      <c r="J26" s="3">
-        <v>0</v>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L26" s="3">
-        <v>0</v>
-      </c>
-      <c r="M26" s="3">
-        <v>0</v>
-      </c>
-      <c r="N26" s="3">
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0</v>
+      </c>
+      <c r="N26" s="2">
         <v>0</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P26" s="3">
+      <c r="P26" s="2">
         <v>0</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R26" s="3">
-        <v>0</v>
-      </c>
-      <c r="S26" s="3">
-        <v>0</v>
-      </c>
-      <c r="T26" s="3">
-        <v>0</v>
-      </c>
-      <c r="U26" s="3">
+      <c r="R26" s="2">
+        <v>0</v>
+      </c>
+      <c r="S26" s="2">
+        <v>0</v>
+      </c>
+      <c r="T26" s="2">
+        <v>0</v>
+      </c>
+      <c r="U26" s="2">
         <v>0</v>
       </c>
       <c r="V26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="W26" s="3">
-        <v>0</v>
-      </c>
-      <c r="X26" s="3">
+      <c r="W26" s="2">
+        <v>0</v>
+      </c>
+      <c r="X26" s="2">
         <v>0</v>
       </c>
       <c r="Y26" s="1" t="s">
@@ -3117,13 +3119,13 @@
       <c r="AA26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB26" s="3">
+      <c r="AB26" s="2">
         <v>0</v>
       </c>
       <c r="AC26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AD26" s="3">
+      <c r="AD26" s="2">
         <v>0</v>
       </c>
       <c r="AE26" s="1" t="s">
@@ -3143,25 +3145,25 @@
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="3">
-        <v>0</v>
-      </c>
-      <c r="C27" s="3">
-        <v>0</v>
-      </c>
-      <c r="D27" s="3">
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
         <v>0</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>0</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="2">
         <v>0</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -3173,19 +3175,19 @@
       <c r="K27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L27" s="3">
+      <c r="L27" s="2">
         <v>0</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N27" s="3">
+      <c r="N27" s="2">
         <v>0</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P27" s="3">
+      <c r="P27" s="2">
         <v>0</v>
       </c>
       <c r="Q27" s="1" t="s">
@@ -3200,7 +3202,7 @@
       <c r="T27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="U27" s="3">
+      <c r="U27" s="2">
         <v>0</v>
       </c>
       <c r="V27" s="1" t="s">
@@ -3209,31 +3211,31 @@
       <c r="W27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X27" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y27" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z27" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA27" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="3">
+      <c r="X27" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="2">
         <v>0</v>
       </c>
       <c r="AC27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AD27" s="3">
+      <c r="AD27" s="2">
         <v>0</v>
       </c>
       <c r="AE27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AF27" s="3">
+      <c r="AF27" s="2">
         <v>0</v>
       </c>
       <c r="AG27" s="1" t="s">
@@ -3247,13 +3249,13 @@
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>0</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -3265,7 +3267,7 @@
       <c r="G28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="2">
         <v>0</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -3274,46 +3276,46 @@
       <c r="J28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K28" s="3">
-        <v>0</v>
-      </c>
-      <c r="L28" s="3">
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2">
         <v>0</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N28" s="3">
+      <c r="N28" s="2">
         <v>0</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P28" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="3">
-        <v>0</v>
-      </c>
-      <c r="R28" s="3">
-        <v>0</v>
-      </c>
-      <c r="S28" s="3">
+      <c r="P28" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>0</v>
+      </c>
+      <c r="R28" s="2">
+        <v>0</v>
+      </c>
+      <c r="S28" s="2">
         <v>0</v>
       </c>
       <c r="T28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="U28" s="3">
-        <v>0</v>
-      </c>
-      <c r="V28" s="3">
+      <c r="U28" s="2">
+        <v>0</v>
+      </c>
+      <c r="V28" s="2">
         <v>0</v>
       </c>
       <c r="W28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X28" s="3">
+      <c r="X28" s="2">
         <v>0</v>
       </c>
       <c r="Y28" s="1" t="s">
@@ -3325,19 +3327,19 @@
       <c r="AA28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB28" s="3">
+      <c r="AB28" s="2">
         <v>0</v>
       </c>
       <c r="AC28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AD28" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE28" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF28" s="3">
+      <c r="AD28" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="2">
         <v>0</v>
       </c>
       <c r="AG28" s="1" t="s">
@@ -3351,34 +3353,34 @@
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="3">
-        <v>0</v>
-      </c>
-      <c r="E29" s="3">
-        <v>0</v>
-      </c>
-      <c r="F29" s="3">
-        <v>0</v>
-      </c>
-      <c r="G29" s="3">
-        <v>0</v>
-      </c>
-      <c r="H29" s="3">
-        <v>0</v>
-      </c>
-      <c r="I29" s="3">
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
         <v>0</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K29" s="2">
         <v>0</v>
       </c>
       <c r="L29" s="1" t="s">
@@ -3387,7 +3389,7 @@
       <c r="M29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N29" s="3">
+      <c r="N29" s="2">
         <v>0</v>
       </c>
       <c r="O29" s="1" t="s">
@@ -3417,19 +3419,19 @@
       <c r="W29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X29" s="3">
+      <c r="X29" s="2">
         <v>0</v>
       </c>
       <c r="Y29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z29" s="3">
+      <c r="Z29" s="2">
         <v>0</v>
       </c>
       <c r="AA29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB29" s="3">
+      <c r="AB29" s="2">
         <v>0</v>
       </c>
       <c r="AC29" s="1" t="s">
@@ -3441,7 +3443,7 @@
       <c r="AE29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AF29" s="3">
+      <c r="AF29" s="2">
         <v>0</v>
       </c>
       <c r="AG29" s="1" t="s">
@@ -3455,7 +3457,7 @@
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -3467,7 +3469,7 @@
       <c r="E30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="2">
         <v>0</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -3482,40 +3484,40 @@
       <c r="J30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K30" s="3">
+      <c r="K30" s="2">
         <v>0</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M30" s="3">
-        <v>0</v>
-      </c>
-      <c r="N30" s="3">
-        <v>0</v>
-      </c>
-      <c r="O30" s="3">
-        <v>0</v>
-      </c>
-      <c r="P30" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="3">
-        <v>0</v>
-      </c>
-      <c r="R30" s="3">
-        <v>0</v>
-      </c>
-      <c r="S30" s="3">
-        <v>0</v>
-      </c>
-      <c r="T30" s="3">
-        <v>0</v>
-      </c>
-      <c r="U30" s="3">
-        <v>0</v>
-      </c>
-      <c r="V30" s="3">
+      <c r="M30" s="2">
+        <v>0</v>
+      </c>
+      <c r="N30" s="2">
+        <v>0</v>
+      </c>
+      <c r="O30" s="2">
+        <v>0</v>
+      </c>
+      <c r="P30" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>0</v>
+      </c>
+      <c r="R30" s="2">
+        <v>0</v>
+      </c>
+      <c r="S30" s="2">
+        <v>0</v>
+      </c>
+      <c r="T30" s="2">
+        <v>0</v>
+      </c>
+      <c r="U30" s="2">
+        <v>0</v>
+      </c>
+      <c r="V30" s="2">
         <v>0</v>
       </c>
       <c r="W30" s="1" t="s">
@@ -3527,25 +3529,25 @@
       <c r="Y30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z30" s="3">
+      <c r="Z30" s="2">
         <v>0</v>
       </c>
       <c r="AA30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB30" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC30" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD30" s="3">
+      <c r="AB30" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="2">
         <v>0</v>
       </c>
       <c r="AE30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AF30" s="3">
+      <c r="AF30" s="2">
         <v>0</v>
       </c>
       <c r="AG30" s="1" t="s">
@@ -3559,40 +3561,40 @@
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="3">
-        <v>0</v>
-      </c>
-      <c r="C31" s="3">
-        <v>0</v>
-      </c>
-      <c r="D31" s="3">
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
         <v>0</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F31" s="3">
-        <v>0</v>
-      </c>
-      <c r="G31" s="3">
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
         <v>0</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I31" s="3">
-        <v>0</v>
-      </c>
-      <c r="J31" s="3">
-        <v>0</v>
-      </c>
-      <c r="K31" s="3">
+      <c r="I31" s="2">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0</v>
+      </c>
+      <c r="K31" s="2">
         <v>0</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M31" s="3">
+      <c r="M31" s="2">
         <v>0</v>
       </c>
       <c r="N31" s="1" t="s">
@@ -3601,7 +3603,7 @@
       <c r="O31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P31" s="3">
+      <c r="P31" s="2">
         <v>0</v>
       </c>
       <c r="Q31" s="1" t="s">
@@ -3613,43 +3615,43 @@
       <c r="S31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T31" s="3">
+      <c r="T31" s="2">
         <v>0</v>
       </c>
       <c r="U31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V31" s="3">
-        <v>0</v>
-      </c>
-      <c r="W31" s="3">
-        <v>0</v>
-      </c>
-      <c r="X31" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y31" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z31" s="3">
+      <c r="V31" s="2">
+        <v>0</v>
+      </c>
+      <c r="W31" s="2">
+        <v>0</v>
+      </c>
+      <c r="X31" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="2">
         <v>0</v>
       </c>
       <c r="AA31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB31" s="3">
+      <c r="AB31" s="2">
         <v>0</v>
       </c>
       <c r="AC31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AD31" s="3">
+      <c r="AD31" s="2">
         <v>0</v>
       </c>
       <c r="AE31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AF31" s="3">
+      <c r="AF31" s="2">
         <v>0</v>
       </c>
       <c r="AG31" s="1" t="s">
@@ -3663,7 +3665,7 @@
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -3675,7 +3677,7 @@
       <c r="E32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="2">
         <v>0</v>
       </c>
       <c r="G32" s="1" t="s">
@@ -3687,7 +3689,7 @@
       <c r="I32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="2">
         <v>0</v>
       </c>
       <c r="K32" s="1" t="s">
@@ -3696,28 +3698,28 @@
       <c r="L32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M32" s="3">
+      <c r="M32" s="2">
         <v>0</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O32" s="3">
-        <v>0</v>
-      </c>
-      <c r="P32" s="3">
+      <c r="O32" s="2">
+        <v>0</v>
+      </c>
+      <c r="P32" s="2">
         <v>0</v>
       </c>
       <c r="Q32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R32" s="3">
+      <c r="R32" s="2">
         <v>0</v>
       </c>
       <c r="S32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T32" s="3">
+      <c r="T32" s="2">
         <v>0</v>
       </c>
       <c r="U32" s="1" t="s">
@@ -3741,19 +3743,19 @@
       <c r="AA32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB32" s="3">
+      <c r="AB32" s="2">
         <v>0</v>
       </c>
       <c r="AC32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AD32" s="3">
+      <c r="AD32" s="2">
         <v>0</v>
       </c>
       <c r="AE32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AF32" s="3">
+      <c r="AF32" s="2">
         <v>0</v>
       </c>
       <c r="AG32" s="1" t="s">
@@ -3767,46 +3769,46 @@
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="3">
-        <v>0</v>
-      </c>
-      <c r="C33" s="3">
-        <v>0</v>
-      </c>
-      <c r="D33" s="3">
-        <v>0</v>
-      </c>
-      <c r="E33" s="3">
-        <v>0</v>
-      </c>
-      <c r="F33" s="3">
-        <v>0</v>
-      </c>
-      <c r="G33" s="3">
-        <v>0</v>
-      </c>
-      <c r="H33" s="3">
-        <v>0</v>
-      </c>
-      <c r="I33" s="3">
-        <v>0</v>
-      </c>
-      <c r="J33" s="3">
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2">
         <v>0</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L33" s="3">
-        <v>0</v>
-      </c>
-      <c r="M33" s="3">
+      <c r="L33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M33" s="2">
         <v>0</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O33" s="3">
+      <c r="O33" s="2">
         <v>0</v>
       </c>
       <c r="P33" s="1" t="s">
@@ -3815,49 +3817,49 @@
       <c r="Q33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R33" s="3">
-        <v>0</v>
-      </c>
-      <c r="S33" s="3">
-        <v>0</v>
-      </c>
-      <c r="T33" s="3">
-        <v>0</v>
-      </c>
-      <c r="U33" s="3">
-        <v>0</v>
-      </c>
-      <c r="V33" s="3">
-        <v>0</v>
-      </c>
-      <c r="W33" s="3">
-        <v>0</v>
-      </c>
-      <c r="X33" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y33" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z33" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA33" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB33" s="3">
+      <c r="R33" s="2">
+        <v>0</v>
+      </c>
+      <c r="S33" s="2">
+        <v>0</v>
+      </c>
+      <c r="T33" s="2">
+        <v>0</v>
+      </c>
+      <c r="U33" s="2">
+        <v>0</v>
+      </c>
+      <c r="V33" s="2">
+        <v>0</v>
+      </c>
+      <c r="W33" s="2">
+        <v>0</v>
+      </c>
+      <c r="X33" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="2">
         <v>0</v>
       </c>
       <c r="AC33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AD33" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE33" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF33" s="3">
+      <c r="AD33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF33" s="2">
         <v>0</v>
       </c>
       <c r="AG33" s="1" t="s">
@@ -3968,86 +3970,6 @@
         <v>0</v>
       </c>
       <c r="AH34" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed made to Maze.csv, adding NUMROWS and COLS, changes to MazeCell and Maze
</commit_message>
<xml_diff>
--- a/Maze.xlsx
+++ b/Maze.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="15">
   <si>
     <t>X</t>
   </si>
@@ -428,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG30" sqref="AG30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,7 +483,7 @@
       <c r="O1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2">
         <v>0</v>
       </c>
       <c r="Q1" s="1" t="s">

</xml_diff>

<commit_message>
Working on the Marker legend
</commit_message>
<xml_diff>
--- a/Maze.xlsx
+++ b/Maze.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="16">
   <si>
     <t>X</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
@@ -428,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG30" sqref="AG30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,7 +486,7 @@
       <c r="O1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="2">
+      <c r="P1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="Q1" s="1" t="s">
@@ -3309,8 +3312,8 @@
       <c r="U28" s="2">
         <v>0</v>
       </c>
-      <c r="V28" s="2">
-        <v>0</v>
+      <c r="V28" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="W28" s="1" t="s">
         <v>0</v>
@@ -3800,7 +3803,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M33" s="2">
         <v>0</v>

</xml_diff>